<commit_message>
Rieseguiti nuovamente i test come da richiesta
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#RSAWEBXX/RSA_Software/MedicalServices/2025.6.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#RSAWEBXX/RSA_Software/MedicalServices/2025.6.0/report-checklist.xlsx
@@ -761,198 +761,6 @@
     <t>subject_application_version: 2025.6.0</t>
   </si>
   <si>
-    <t>2025-04-23T16:57:05Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:09Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:13Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:17Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:21Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:24Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:28Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:31Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:36Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:40Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:43Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:46Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:50Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:54Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:57:58Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:58:02Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:58:06Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:58:10Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:58:13Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:58:18Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:58:25Z</t>
-  </si>
-  <si>
-    <t>2025-04-23T16:58:29Z</t>
-  </si>
-  <si>
-    <t>d14bd81a57151c193ab6d645f7966bd8</t>
-  </si>
-  <si>
-    <t>5d3db2936524c824c3ff95466dc98e6c</t>
-  </si>
-  <si>
-    <t>aca07480e366d734391607501dfb77ac</t>
-  </si>
-  <si>
-    <t>10c6413dbfed8bb3c88e175bd744c3c6</t>
-  </si>
-  <si>
-    <t>6276e5d11d122135921fe578d22ab245</t>
-  </si>
-  <si>
-    <t>acccce1e8056cda4e5d60f0beae17ebd</t>
-  </si>
-  <si>
-    <t>46f8426737c0b6680a75866c36f44b77</t>
-  </si>
-  <si>
-    <t>809eed45348295d999822906e8cf2e06</t>
-  </si>
-  <si>
-    <t>a8b556df04f5936c31d3bd4431b51149</t>
-  </si>
-  <si>
-    <t>e57566954873d07c6a108258e9b5e2e3</t>
-  </si>
-  <si>
-    <t>227a6994389da3d02cee683223e30b29</t>
-  </si>
-  <si>
-    <t>3210dda3fb1abb80879fb5481a94ecfd</t>
-  </si>
-  <si>
-    <t>0c3e0f1271384a92836a757d4ae85816</t>
-  </si>
-  <si>
-    <t>bb872db90ef51416b74aface65ad24b8</t>
-  </si>
-  <si>
-    <t>32012f9164f28a932b3cd0cd31edc299</t>
-  </si>
-  <si>
-    <t>f9c516eb3cbbac5f6abe08150d4ef868</t>
-  </si>
-  <si>
-    <t>bd461fcb6d23d2dbc92733cd9d24a8f9</t>
-  </si>
-  <si>
-    <t>23a325d2b56db5ca9f785445f04d2c3a</t>
-  </si>
-  <si>
-    <t>9001650f0956d64f431803552fa981fa</t>
-  </si>
-  <si>
-    <t>eefe6da26a1acf4d233a6bce4ce7f6c6</t>
-  </si>
-  <si>
-    <t>bfcb1e316d078bddfcf970806c1a5069</t>
-  </si>
-  <si>
-    <t>2df6b465259f9d3c23abc0ac168da17f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.41310c97e2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.43fb8a7b36^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.a206aa308f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.ced504987b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.3ff4c75c5a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.d67f44c3f7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.89bea28d62^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.73b79703b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.71d5e49257^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.9f2a1e270e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.d151f03780^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.094be92226^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.cab490bba4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.43fc26f393^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.7d8a0f0a9c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.3c93e2f4c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.14e5dffe9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.d144e3b2c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.6424c070fd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.990042d197^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Per poter ricreare questo errore è stata modificata temporaneamente la funzione di generazione dell’XML e tolto il controllo di validazione tramite file XSD. Normalmente questa situazione non si potrebbe mai verificare perché il campo codice fiscale è sempre memorizzato in maiuscolo</t>
   </si>
   <si>
@@ -960,6 +768,198 @@
   </si>
   <si>
     <t>Per poter ricreare questo errore è stata modificata temporaneamente la funzione di generazione dell’XML e tolto il controllo di validazione tramite file XSD. Normalmente questa situazione non si potrebbe mai verificare perché la presenza del campo viene verificata prima dell'invio.</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:30:52Z</t>
+  </si>
+  <si>
+    <t>040893f7eab1b5b71b96e043eaae4ce4</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:02Z</t>
+  </si>
+  <si>
+    <t>05aa9475d1255e1091e6e21043878526</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:05Z</t>
+  </si>
+  <si>
+    <t>288c8771d42e7262664c47ddc2eabcff</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.00eb410c1a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:09Z</t>
+  </si>
+  <si>
+    <t>695b59692814539a59ad0bcef216fa31</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.68ddfa9ad5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:13Z</t>
+  </si>
+  <si>
+    <t>e115d6b3f1947d18b105fee59906c679</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.c8bde5ff00^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:17Z</t>
+  </si>
+  <si>
+    <t>c0c176586ad24581ebef05160a2143a1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.7b3c67f14a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:21Z</t>
+  </si>
+  <si>
+    <t>59e9fa80881b7951c27c912be4fdea9a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.569cbca794^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:25Z</t>
+  </si>
+  <si>
+    <t>7a32d91c957b777522559a49cdc5d7c1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.aefb8ea23e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:29Z</t>
+  </si>
+  <si>
+    <t>94a78b315362cf3ee597a7de91446b73</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.4ddea6e582^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:35Z</t>
+  </si>
+  <si>
+    <t>a9e14c0cbe1b36c139fca7798e4b322a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.e501e9aa6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:39Z</t>
+  </si>
+  <si>
+    <t>2e178e8035eebdc267bf242d93bde7f5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.32df656c91^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:43Z</t>
+  </si>
+  <si>
+    <t>fab2154704e3a83a19f8ccb6e9998176</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.741db9c540^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:47Z</t>
+  </si>
+  <si>
+    <t>fa32aebe5d22b4930b7168a8e51e2845</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.60b6fe83ef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:51Z</t>
+  </si>
+  <si>
+    <t>df6b2681537aeb1469646a81dcde0d62</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.f5ba5cd458^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:55Z</t>
+  </si>
+  <si>
+    <t>38f0264bfdf3ee8d4bba68966d841e54</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.6cac6b41a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:31:59Z</t>
+  </si>
+  <si>
+    <t>f268c856ef4be6fe70166d1d8d202ccf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.d2b1461257^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:32:03Z</t>
+  </si>
+  <si>
+    <t>b77e6cc09aa21dbd860d53fd9a1ee24a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.b86740564d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:32:07Z</t>
+  </si>
+  <si>
+    <t>ffa0382c9006e2e805d2b81ff7886aa4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.1af69824d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:32:11Z</t>
+  </si>
+  <si>
+    <t>96ecc2425175a97823a7862f378fcd57</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.d86aa599af^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:32:16Z</t>
+  </si>
+  <si>
+    <t>1649499c4aeba82ad72bf1e3930a36a6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.37c24f92f7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:32:20Z</t>
+  </si>
+  <si>
+    <t>7083e8e7abed78ed1314a548ed081add</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.0485520b9f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-07T09:32:24Z</t>
+  </si>
+  <si>
+    <t>2cadb1d6bc218ab8fff37623768f0eb6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed1012189d6a9a56fe3c1c519ea594828420082121fb127aecb0138ffb5f12e7.75a17283bf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2995,10 +2995,10 @@
   <dimension ref="A1:W597"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3007,10 +3007,10 @@
     <col min="2" max="2" width="46.81640625" customWidth="1"/>
     <col min="3" max="3" width="20.1796875" customWidth="1"/>
     <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="69" customWidth="1"/>
-    <col min="6" max="6" width="23.26953125" customWidth="1"/>
-    <col min="7" max="7" width="30.6328125" customWidth="1"/>
-    <col min="8" max="8" width="22.08984375" customWidth="1"/>
+    <col min="5" max="5" width="47.7265625" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="25.81640625" customWidth="1"/>
+    <col min="8" max="8" width="40.453125" customWidth="1"/>
     <col min="9" max="9" width="72.08984375" customWidth="1"/>
     <col min="10" max="10" width="27.1796875" customWidth="1"/>
     <col min="11" max="11" width="43.26953125" customWidth="1"/>
@@ -3219,7 +3219,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="1:23" s="18" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:23" s="18" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="31">
         <v>32</v>
       </c>
@@ -3307,13 +3307,13 @@
         <v>42</v>
       </c>
       <c r="F10" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="I10" s="37" t="s">
         <v>142</v>
@@ -3353,7 +3353,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="31">
         <v>40</v>
       </c>
@@ -3370,13 +3370,13 @@
         <v>47</v>
       </c>
       <c r="F11" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="I11" s="37" t="s">
         <v>142</v>
@@ -3416,7 +3416,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="31">
         <v>48</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>89</v>
       </c>
       <c r="F12" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
@@ -3471,7 +3471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="31">
         <v>152</v>
       </c>
@@ -3488,16 +3488,16 @@
         <v>108</v>
       </c>
       <c r="F13" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="I13" s="37" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="J13" s="29" t="s">
         <v>49</v>
@@ -3528,13 +3528,13 @@
       <c r="T13" s="29"/>
       <c r="U13" s="34"/>
       <c r="V13" s="35" t="s">
-        <v>234</v>
+        <v>170</v>
       </c>
       <c r="W13" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="31">
         <v>154</v>
       </c>
@@ -3551,16 +3551,16 @@
         <v>109</v>
       </c>
       <c r="F14" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
       <c r="J14" s="29" t="s">
         <v>49</v>
@@ -3591,13 +3591,13 @@
       <c r="T14" s="29"/>
       <c r="U14" s="34"/>
       <c r="V14" s="35" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
       <c r="W14" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="31">
         <v>155</v>
       </c>
@@ -3614,16 +3614,16 @@
         <v>110</v>
       </c>
       <c r="F15" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="I15" s="37" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="J15" s="29" t="s">
         <v>49</v>
@@ -3654,13 +3654,13 @@
       <c r="T15" s="29"/>
       <c r="U15" s="34"/>
       <c r="V15" s="35" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
       <c r="W15" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="31">
         <v>156</v>
       </c>
@@ -3677,16 +3677,16 @@
         <v>111</v>
       </c>
       <c r="F16" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="I16" s="37" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="J16" s="29" t="s">
         <v>49</v>
@@ -3721,7 +3721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="31">
         <v>158</v>
       </c>
@@ -3738,16 +3738,16 @@
         <v>112</v>
       </c>
       <c r="F17" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I17" s="37" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="J17" s="29" t="s">
         <v>49</v>
@@ -3782,7 +3782,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="31">
         <v>159</v>
       </c>
@@ -3799,16 +3799,16 @@
         <v>57</v>
       </c>
       <c r="F18" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="J18" s="29" t="s">
         <v>49</v>
@@ -3843,7 +3843,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="31">
         <v>160</v>
       </c>
@@ -3860,16 +3860,16 @@
         <v>59</v>
       </c>
       <c r="F19" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I19" s="37" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>49</v>
@@ -3904,7 +3904,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="31">
         <v>161</v>
       </c>
@@ -3921,16 +3921,16 @@
         <v>99</v>
       </c>
       <c r="F20" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I20" s="37" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>49</v>
@@ -3961,13 +3961,13 @@
       <c r="T20" s="29"/>
       <c r="U20" s="34"/>
       <c r="V20" s="35" t="s">
-        <v>236</v>
+        <v>172</v>
       </c>
       <c r="W20" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="31">
         <v>162</v>
       </c>
@@ -3984,16 +3984,16 @@
         <v>100</v>
       </c>
       <c r="F21" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="H21" s="33" t="s">
         <v>202</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="J21" s="29" t="s">
         <v>49</v>
@@ -4024,13 +4024,13 @@
       <c r="T21" s="29"/>
       <c r="U21" s="34"/>
       <c r="V21" s="35" t="s">
-        <v>236</v>
+        <v>172</v>
       </c>
       <c r="W21" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="31">
         <v>163</v>
       </c>
@@ -4047,16 +4047,16 @@
         <v>101</v>
       </c>
       <c r="F22" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="J22" s="29" t="s">
         <v>49</v>
@@ -4091,7 +4091,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="31">
         <v>164</v>
       </c>
@@ -4108,16 +4108,16 @@
         <v>102</v>
       </c>
       <c r="F23" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="J23" s="29" t="s">
         <v>49</v>
@@ -4152,7 +4152,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="31">
         <v>165</v>
       </c>
@@ -4169,16 +4169,16 @@
         <v>103</v>
       </c>
       <c r="F24" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="I24" s="37" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="J24" s="29" t="s">
         <v>49</v>
@@ -4213,7 +4213,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="31">
         <v>166</v>
       </c>
@@ -4230,16 +4230,16 @@
         <v>104</v>
       </c>
       <c r="F25" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="J25" s="29" t="s">
         <v>49</v>
@@ -4274,7 +4274,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="31">
         <v>167</v>
       </c>
@@ -4291,16 +4291,16 @@
         <v>105</v>
       </c>
       <c r="F26" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="I26" s="37" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J26" s="29" t="s">
         <v>49</v>
@@ -4335,7 +4335,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="31">
         <v>168</v>
       </c>
@@ -4352,16 +4352,16 @@
         <v>106</v>
       </c>
       <c r="F27" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>186</v>
+        <v>219</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="I27" s="37" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J27" s="29" t="s">
         <v>49</v>
@@ -4396,7 +4396,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="31">
         <v>169</v>
       </c>
@@ -4413,16 +4413,16 @@
         <v>107</v>
       </c>
       <c r="F28" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="I28" s="37" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="J28" s="29" t="s">
         <v>49</v>
@@ -4457,7 +4457,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="31">
         <v>448</v>
       </c>
@@ -4474,16 +4474,16 @@
         <v>120</v>
       </c>
       <c r="F29" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
       <c r="H29" s="33" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="J29" s="29" t="s">
         <v>49</v>
@@ -4504,7 +4504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="31">
         <v>449</v>
       </c>
@@ -4521,16 +4521,16 @@
         <v>121</v>
       </c>
       <c r="F30" s="33">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="H30" s="33" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="I30" s="37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J30" s="29" t="s">
         <v>49</v>
@@ -4551,7 +4551,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="41">
         <v>461</v>
       </c>
@@ -4568,16 +4568,16 @@
         <v>122</v>
       </c>
       <c r="F31" s="44">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="H31" s="43" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="I31" s="43" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J31" s="41" t="s">
         <v>49</v>
@@ -4612,7 +4612,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:23" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="41">
         <v>468</v>
       </c>
@@ -4629,16 +4629,16 @@
         <v>129</v>
       </c>
       <c r="F32" s="44">
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="G32" s="41" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="H32" s="43" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="I32" s="43" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J32" s="41" t="s">
         <v>49</v>

</xml_diff>